<commit_message>
Edit system level testing spreadsheet
</commit_message>
<xml_diff>
--- a/src/System Level Testing/System Level Testing - Rizky Abraham.xlsx
+++ b/src/System Level Testing/System Level Testing - Rizky Abraham.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\00.2019 Spring\CIT 360\Week 3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rizky\Documents\NetBeansProjects\CIT360\src\System Level Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A91636F5-4546-4C80-ADE5-83B25C2B47AF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E31E263-AB70-4602-A9B0-362CF20198A4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="675" windowWidth="19440" windowHeight="15000" xr2:uid="{913333B8-A57B-4672-91CA-3F7A4FA796F1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{913333B8-A57B-4672-91CA-3F7A4FA796F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
   <si>
     <t>Test Case</t>
   </si>
@@ -133,6 +133,21 @@
   </si>
   <si>
     <t>All information is displayed correctly</t>
+  </si>
+  <si>
+    <t>User chooses to do another transaction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Screen should display main menu screen </t>
+  </si>
+  <si>
+    <t>User choosed to end transaction</t>
+  </si>
+  <si>
+    <t>Quit menu screen should be displayed. System will asked user to remove card first, then cash if desired, and receipt in the end.</t>
+  </si>
+  <si>
+    <t>All information is displayed correctly, sequence is followed correctly</t>
   </si>
 </sst>
 </file>
@@ -204,7 +219,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -312,11 +327,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -352,17 +378,29 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -474,6 +512,75 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -514,75 +621,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <name val="Calibri Light"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <name val="Calibri Light"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </font>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -597,9 +635,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1B8E7D83-E896-4F69-BF23-2799CA7FF35C}" name="Table1" displayName="Table1" ref="A4:E12" totalsRowShown="0" headerRowDxfId="4" dataDxfId="6" headerRowBorderDxfId="8" tableBorderDxfId="9" totalsRowBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1B8E7D83-E896-4F69-BF23-2799CA7FF35C}" name="Table1" displayName="Table1" ref="A4:E14" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6" totalsRowBorderDxfId="5">
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{C71CA981-9FC2-4ECD-806F-EF5FE672C41C}" name="#" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{C71CA981-9FC2-4ECD-806F-EF5FE672C41C}" name="#" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{FD006FD0-30DF-4C65-ABFD-AC9E49AC001C}" name="Test Case" dataDxfId="3"/>
     <tableColumn id="3" xr3:uid="{54C9C268-03D9-4864-A134-466D276E04EB}" name="Expected Result" dataDxfId="2"/>
     <tableColumn id="4" xr3:uid="{CD18485D-A719-4516-8D46-299EAC28B98D}" name="Actual Result" dataDxfId="1"/>
@@ -906,10 +944,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58B81F1D-F9B3-4B99-A5F3-01D1EF8A242F}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -923,11 +961,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
       <c r="D1" s="12" t="s">
         <v>9</v>
       </c>
@@ -970,7 +1008,7 @@
       <c r="D5" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="13" t="s">
         <v>5</v>
       </c>
     </row>
@@ -987,7 +1025,7 @@
       <c r="D6" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="14" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1004,7 +1042,7 @@
       <c r="D7" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="13" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1021,41 +1059,41 @@
       <c r="D8" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="14" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>5</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>24</v>
+      <c r="B9" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="E9" s="14" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>6</v>
       </c>
-      <c r="B10" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" s="15" t="s">
+      <c r="B10" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="13" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1072,12 +1110,12 @@
       <c r="D11" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="13" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
+      <c r="A12" s="6">
         <v>8</v>
       </c>
       <c r="B12" s="11" t="s">
@@ -1089,7 +1127,41 @@
       <c r="D12" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="E12" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>9</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="17">
+        <v>10</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="19" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>